<commit_message>
a sheet to try excels paste special menu
</commit_message>
<xml_diff>
--- a/Excel Obstacle Course 2 MAC XTimer.xlsx
+++ b/Excel Obstacle Course 2 MAC XTimer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imac/Library/Containers/com.apple.iWork.Pages/Data/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RAMANA03/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72DD8AFD-FDEB-C449-B194-8C89C103B0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57C4E75-6DF6-4E4F-95C2-B504B388E832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A51B3495-FB35-4BD8-B569-4CA137411D06}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="9" xr2:uid="{A51B3495-FB35-4BD8-B569-4CA137411D06}"/>
   </bookViews>
   <sheets>
     <sheet name="Creator's Message" sheetId="14" r:id="rId1"/>
@@ -22,13 +22,15 @@
     <sheet name="Font size" sheetId="7" r:id="rId7"/>
     <sheet name="formatting 2" sheetId="6" r:id="rId8"/>
     <sheet name="format painting" sheetId="16" r:id="rId9"/>
-    <sheet name="find and replace" sheetId="3" r:id="rId10"/>
-    <sheet name="auto filter" sheetId="2" r:id="rId11"/>
-    <sheet name="FINAL" sheetId="9" r:id="rId12"/>
+    <sheet name="paste special" sheetId="17" r:id="rId10"/>
+    <sheet name="find and replace" sheetId="3" r:id="rId11"/>
+    <sheet name="auto filter" sheetId="2" r:id="rId12"/>
+    <sheet name="FINAL" sheetId="9" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'auto filter'!$A$1:$A$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'auto filter'!$A$1:$A$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Font size'!$A$1:$A$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'paste special'!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="59">
   <si>
     <t>A</t>
   </si>
@@ -235,12 +237,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="mm:ss.0;@"/>
-    <numFmt numFmtId="165" formatCode="mm:ss.000"/>
-    <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="mm:ss.0;@"/>
+    <numFmt numFmtId="166" formatCode="mm:ss.000"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,8 +354,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +400,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -634,7 +649,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -669,7 +684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -680,13 +695,13 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -727,6 +742,9 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
@@ -735,7 +753,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -755,6 +773,35 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -903,6 +950,213 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>511176</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{702C245F-D8FE-4241-A8F4-99394806F48F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791200" y="101600"/>
+          <a:ext cx="7102476" cy="3086100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Copy all cells from A1:E24</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> to A28:E51 without any format</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Hint: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Hold CTRL, tap A; Cmd C</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>move to A28; </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Cmd + Opt + V</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Select values</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>612774</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -1039,7 +1293,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1259,7 +1513,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1849,8 +2103,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9020175" y="190500"/>
-          <a:ext cx="6467475" cy="2076450"/>
+          <a:off x="4305300" y="190500"/>
+          <a:ext cx="7102475" cy="2066925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2047,8 +2301,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6134100" y="0"/>
-          <a:ext cx="6362699" cy="2190750"/>
+          <a:off x="6769100" y="0"/>
+          <a:ext cx="6997699" cy="2190750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3471,9 +3725,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3511,7 +3765,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3617,7 +3871,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3759,7 +4013,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3786,6 +4040,197 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8B8C03-FC96-DE46-87C8-8CDFC4EBA41D}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="C2" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="C4" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="E7" s="46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="C9" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="E10" s="46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="D13" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="E15" s="46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="C16" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="C18" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="E19" s="46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="C22" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="E23" s="46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2954D1-10B9-4D9A-BC79-4E7EBD7A50DB}">
   <dimension ref="B3:H20"/>
   <sheetViews>
@@ -4144,7 +4589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE56F37-E1A1-4AC9-AEEF-72A6CDC847E1}">
   <dimension ref="A1:A36"/>
   <sheetViews>
@@ -4339,7 +4784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB67D47-939A-4EDE-ACE8-5719E8BC6DCB}">
   <dimension ref="A2:L13"/>
   <sheetViews>
@@ -4475,7 +4920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF69F03-2891-468A-AB81-3AFCC0BCB467}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4774,7 +5219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161508D5-A8E7-41FE-BAE4-32741EDA573B}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7150,7 +7597,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>